<commit_message>
updates to data pipeline
</commit_message>
<xml_diff>
--- a/Recipes-Orange.xlsx
+++ b/Recipes-Orange.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/raphael_caillon_sap_com/Documents/iLab/Recipe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/raphael_caillon_sap_com/Documents/iLab/Recipe/PLMcollectors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_108216D41958DB57342F6FEA1FB1693F28017D7F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{786C5432-7612-954A-BE79-25E54441367A}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_108216D41958DB57342F6FEA1FB1693F28017D7F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDE8A82A-F277-F04E-90BD-2334571C7DBA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7518,7 +7518,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>